<commit_message>
implementação: data automatica, salvar titulo arquivo.
</commit_message>
<xml_diff>
--- a/modelo/modOrd.xlsx
+++ b/modelo/modOrd.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shemu\Documents\meu github\pyGensto\modelo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21EA079F-898E-4305-8FA6-0F3F807A34FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADC60F21-4EC9-4C62-8656-DB90273D00FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{1D20669B-06E3-480B-A3BB-DEB81C99BCEC}"/>
   </bookViews>
@@ -260,7 +260,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -280,9 +280,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -296,8 +293,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -314,13 +320,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -641,26 +658,26 @@
   <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.5703125" customWidth="1"/>
     <col min="2" max="2" width="6.7109375" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="22"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="24"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
@@ -669,40 +686,40 @@
       <c r="D2" s="7"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="10" t="s">
+      <c r="B3" s="27"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="2"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="28"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="12"/>
+      <c r="A4" s="11"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="11"/>
       <c r="E4" s="5"/>
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="28"/>
       <c r="D5" s="10"/>
       <c r="E5" s="1"/>
       <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="12"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="12"/>
+      <c r="A6" s="11"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="11"/>
       <c r="E6" s="5"/>
       <c r="F6" s="6"/>
     </row>
@@ -713,14 +730,14 @@
       <c r="D7" s="9"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="20" t="s">
+      <c r="A8" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="22"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="24"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="9"/>
@@ -729,62 +746,54 @@
       <c r="D9" s="9"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="10" t="s">
+      <c r="B10" s="27"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="1"/>
-      <c r="F10" s="2"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="32"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="12"/>
+      <c r="A11" s="11"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="11"/>
       <c r="E11" s="5"/>
       <c r="F11" s="6"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="2"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="12"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="6"/>
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="25" t="s">
+      <c r="A14" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="25"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="25" t="s">
+      <c r="A15" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="19"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="27"/>
+      <c r="B15" s="30"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
@@ -793,14 +802,14 @@
       <c r="D16" s="7"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="20" t="s">
+      <c r="A17" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="21"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="22"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="24"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
@@ -809,187 +818,192 @@
       <c r="D18" s="7"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="13" t="s">
         <v>9</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="23" t="s">
+      <c r="C19" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="D19" s="24"/>
-      <c r="E19" s="23" t="s">
+      <c r="D19" s="26"/>
+      <c r="E19" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="F19" s="24"/>
+      <c r="F19" s="26"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="15"/>
-      <c r="B20" s="16"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="17"/>
+      <c r="A20" s="14"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="16"/>
       <c r="E20" s="5"/>
       <c r="F20" s="6"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="15"/>
-      <c r="B21" s="16"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="17"/>
+      <c r="A21" s="14"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="16"/>
       <c r="E21" s="5"/>
       <c r="F21" s="6"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="15"/>
-      <c r="B22" s="16"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="17"/>
+      <c r="A22" s="14"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="16"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="15"/>
-      <c r="B23" s="16"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="17"/>
+      <c r="A23" s="14"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="16"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="15"/>
-      <c r="B24" s="16"/>
-      <c r="C24" s="16"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="17"/>
+      <c r="A24" s="14"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="16"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="15"/>
-      <c r="B25" s="16"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="17"/>
+      <c r="A25" s="14"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="16"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="15"/>
-      <c r="B26" s="16"/>
-      <c r="C26" s="16"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="17"/>
+      <c r="A26" s="14"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="16"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="15"/>
-      <c r="B27" s="16"/>
-      <c r="C27" s="16"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="17"/>
+      <c r="A27" s="14"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="16"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="15"/>
-      <c r="B28" s="16"/>
-      <c r="C28" s="16"/>
-      <c r="D28" s="17"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="17"/>
+      <c r="A28" s="14"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="16"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="15"/>
-      <c r="B29" s="16"/>
-      <c r="C29" s="16"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="17"/>
+      <c r="A29" s="14"/>
+      <c r="B29" s="15"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="16"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="15"/>
-      <c r="B30" s="16"/>
-      <c r="C30" s="16"/>
-      <c r="D30" s="17"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="17"/>
+      <c r="A30" s="14"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="16"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="15"/>
-      <c r="B31" s="16"/>
-      <c r="C31" s="16"/>
-      <c r="D31" s="17"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="17"/>
+      <c r="A31" s="14"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="17"/>
+      <c r="F31" s="16"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="15"/>
-      <c r="B32" s="16"/>
-      <c r="C32" s="16"/>
-      <c r="D32" s="17"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="17"/>
+      <c r="A32" s="14"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="17"/>
+      <c r="F32" s="16"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="15"/>
-      <c r="B33" s="16"/>
-      <c r="C33" s="16"/>
-      <c r="D33" s="17"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="17"/>
+      <c r="A33" s="14"/>
+      <c r="B33" s="15"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="17"/>
+      <c r="F33" s="16"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="15"/>
-      <c r="B34" s="16"/>
-      <c r="C34" s="16"/>
-      <c r="D34" s="17"/>
+      <c r="A34" s="14"/>
+      <c r="B34" s="15"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="16"/>
       <c r="E34" s="5"/>
       <c r="F34" s="6"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="15"/>
-      <c r="B35" s="16"/>
-      <c r="C35" s="16"/>
-      <c r="D35" s="17"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="17"/>
+      <c r="A35" s="14"/>
+      <c r="B35" s="15"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="16"/>
+      <c r="E35" s="17"/>
+      <c r="F35" s="16"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="15"/>
-      <c r="B36" s="16"/>
-      <c r="C36" s="16"/>
-      <c r="D36" s="17"/>
+      <c r="A36" s="14"/>
+      <c r="B36" s="15"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="16"/>
       <c r="E36" s="5"/>
       <c r="F36" s="6"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="15"/>
-      <c r="B37" s="16"/>
-      <c r="C37" s="16"/>
-      <c r="D37" s="17"/>
+      <c r="A37" s="14"/>
+      <c r="B37" s="15"/>
+      <c r="C37" s="15"/>
+      <c r="D37" s="16"/>
       <c r="F37" s="3"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="15"/>
-      <c r="B38" s="16"/>
-      <c r="C38" s="16"/>
-      <c r="D38" s="17"/>
-      <c r="E38" s="18"/>
-      <c r="F38" s="17"/>
+      <c r="A38" s="14"/>
+      <c r="B38" s="15"/>
+      <c r="C38" s="15"/>
+      <c r="D38" s="16"/>
+      <c r="E38" s="17"/>
+      <c r="F38" s="16"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="15"/>
-      <c r="B39" s="16"/>
+      <c r="A39" s="14"/>
+      <c r="B39" s="15"/>
       <c r="C39" s="4"/>
       <c r="D39" s="6"/>
       <c r="E39" s="5"/>
       <c r="F39" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="10">
     <mergeCell ref="A17:F17"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A8:F8"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="E19:F19"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="B5:C5"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" r:id="rId1"/>

</xml_diff>